<commit_message>
Revert "fix bug kdr004"
This reverts commit 310accc4e7d7adc95c845b456270c5e4489ae59b.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR004_template.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR004_template.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03.Source\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7815"/>
   </bookViews>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -465,10 +460,13 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
@@ -589,6 +587,9 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -600,18 +601,6 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -663,6 +652,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -674,9 +675,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -939,423 +937,484 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="9.75"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="22.25" style="1" customWidth="1"/>
-    <col min="3" max="7" width="5.875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="2.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.125" style="1" customWidth="1"/>
-    <col min="10" max="19" width="7.875" style="2" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="3.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.25" style="2" customWidth="1"/>
+    <col min="3" max="7" width="5.875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="5.125" style="2" customWidth="1"/>
+    <col min="10" max="19" width="7.875" style="3" customWidth="1"/>
+    <col min="20" max="20" width="9" style="1"/>
+    <col min="21" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="50"/>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-    </row>
-    <row r="2" spans="1:19" ht="11.25" customHeight="1">
-      <c r="A2" s="54"/>
-      <c r="B2" s="56"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="62"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="45"/>
-    </row>
-    <row r="3" spans="1:19" ht="14.25" customHeight="1">
-      <c r="A3" s="55"/>
-      <c r="B3" s="57"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="61"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="48"/>
-      <c r="O3" s="48"/>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-      <c r="S3" s="46"/>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="52"/>
-      <c r="R4" s="52"/>
-      <c r="S4" s="53"/>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="41"/>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="42"/>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="37"/>
-      <c r="K7" s="37"/>
-      <c r="L7" s="37"/>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="37"/>
-      <c r="P7" s="37"/>
-      <c r="Q7" s="37"/>
-      <c r="R7" s="37"/>
-      <c r="S7" s="43"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="28"/>
-      <c r="P8" s="28"/>
-      <c r="Q8" s="28"/>
-      <c r="R8" s="28"/>
-      <c r="S8" s="42"/>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="37"/>
-      <c r="K9" s="37"/>
-      <c r="L9" s="37"/>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37"/>
-      <c r="O9" s="37"/>
-      <c r="P9" s="37"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="43"/>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="44"/>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37"/>
-      <c r="O11" s="37"/>
-      <c r="P11" s="37"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="43"/>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="28"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="42"/>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="37"/>
-      <c r="K13" s="37"/>
-      <c r="L13" s="37"/>
-      <c r="M13" s="37"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="37"/>
-      <c r="P13" s="37"/>
-      <c r="Q13" s="37"/>
-      <c r="R13" s="37"/>
-      <c r="S13" s="43"/>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="10"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="28"/>
-      <c r="P14" s="28"/>
-      <c r="Q14" s="28"/>
-      <c r="R14" s="28"/>
-      <c r="S14" s="42"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37"/>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="43"/>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
-      <c r="L16" s="28"/>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="28"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="28"/>
-      <c r="S16" s="42"/>
-    </row>
-    <row r="17" spans="1:19">
-      <c r="A17" s="29"/>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="30"/>
-      <c r="L17" s="30"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="30"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="30"/>
-      <c r="S17" s="30"/>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="33"/>
-      <c r="S19" s="33"/>
+    <row r="1" spans="1:20" ht="14.25" customHeight="1">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+    </row>
+    <row r="2" spans="1:20" ht="11.25" customHeight="1">
+      <c r="A2" s="52"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="33"/>
+    </row>
+    <row r="3" spans="1:20" ht="14.25" customHeight="1">
+      <c r="A3" s="53"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="33"/>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="49"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="M4" s="50"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="50"/>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="51"/>
+      <c r="T4" s="33"/>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="43"/>
+      <c r="T5" s="33"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="33"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="38"/>
+      <c r="Q7" s="38"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="33"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="33"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="38"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="33"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="46"/>
+      <c r="T10" s="33"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="38"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="33"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="44"/>
+      <c r="T12" s="33"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="38"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="33"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="44"/>
+      <c r="T14" s="33"/>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
+      <c r="P15" s="38"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="33"/>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="44"/>
+      <c r="T16" s="33"/>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
+      <c r="L17" s="31"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="33"/>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="33"/>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="34"/>
+      <c r="T19" s="33"/>
+    </row>
+    <row r="20" spans="1:20" s="1" customFormat="1">
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="42"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="42"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="42"/>
+      <c r="R20" s="42"/>
+      <c r="S20" s="42"/>
+    </row>
+    <row r="21" spans="1:20" s="1" customFormat="1">
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="42"/>
+    </row>
+    <row r="22" spans="1:20" s="1" customFormat="1">
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="A4:S4"/>
@@ -1372,12 +1431,6 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.31496062992126"/>

</xml_diff>

<commit_message>
Revert "Revert "fix bug kdr004""
This reverts commit 0d7b4932194d11d29d6dc42f821d1c3dcab6247b.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR004_template.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KDR004_template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\03.Source\UniversalK\nts.uk\uk.at\at.file\nts.uk.file.at.infra\src\main\resources\report\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7815"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -460,13 +465,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
@@ -587,9 +589,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -601,6 +600,18 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="31" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
@@ -652,18 +663,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -675,6 +674,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -937,484 +939,423 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="145" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="9.75"/>
   <cols>
-    <col min="1" max="1" width="3.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.25" style="2" customWidth="1"/>
-    <col min="3" max="7" width="5.875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="2.5" style="2" customWidth="1"/>
-    <col min="9" max="9" width="5.125" style="2" customWidth="1"/>
-    <col min="10" max="19" width="7.875" style="3" customWidth="1"/>
-    <col min="20" max="20" width="9" style="1"/>
-    <col min="21" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="3.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.25" style="1" customWidth="1"/>
+    <col min="3" max="7" width="5.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="2.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.125" style="1" customWidth="1"/>
+    <col min="10" max="19" width="7.875" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-    </row>
-    <row r="2" spans="1:20" ht="11.25" customHeight="1">
-      <c r="A2" s="52"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="62"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="33"/>
-    </row>
-    <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="53"/>
-      <c r="B3" s="55"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="33"/>
-    </row>
-    <row r="4" spans="1:20">
-      <c r="A4" s="49"/>
-      <c r="B4" s="50"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="50"/>
-      <c r="K4" s="50"/>
-      <c r="L4" s="50"/>
-      <c r="M4" s="50"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="50"/>
-      <c r="P4" s="50"/>
-      <c r="Q4" s="50"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="33"/>
-    </row>
-    <row r="5" spans="1:20">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="43"/>
-      <c r="T5" s="33"/>
-    </row>
-    <row r="6" spans="1:20">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="29"/>
-      <c r="R6" s="29"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="33"/>
-    </row>
-    <row r="7" spans="1:20">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="33"/>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="29"/>
-      <c r="L8" s="29"/>
-      <c r="M8" s="29"/>
-      <c r="N8" s="29"/>
-      <c r="O8" s="29"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="29"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="33"/>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="17"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="38"/>
-      <c r="Q9" s="38"/>
-      <c r="R9" s="38"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="33"/>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
-      <c r="N10" s="40"/>
-      <c r="O10" s="40"/>
-      <c r="P10" s="40"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="40"/>
-      <c r="S10" s="46"/>
-      <c r="T10" s="33"/>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="38"/>
-      <c r="Q11" s="38"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="33"/>
-    </row>
-    <row r="12" spans="1:20">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="36"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="44"/>
-      <c r="T12" s="33"/>
-    </row>
-    <row r="13" spans="1:20">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="38"/>
-      <c r="P13" s="38"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="33"/>
-    </row>
-    <row r="14" spans="1:20">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="29"/>
-      <c r="O14" s="29"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="29"/>
-      <c r="R14" s="29"/>
-      <c r="S14" s="44"/>
-      <c r="T14" s="33"/>
-    </row>
-    <row r="15" spans="1:20">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="38"/>
-      <c r="P15" s="38"/>
-      <c r="Q15" s="38"/>
-      <c r="R15" s="38"/>
-      <c r="S15" s="45"/>
-      <c r="T15" s="33"/>
-    </row>
-    <row r="16" spans="1:20">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-      <c r="N16" s="29"/>
-      <c r="O16" s="29"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="29"/>
-      <c r="R16" s="29"/>
-      <c r="S16" s="44"/>
-      <c r="T16" s="33"/>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
-      <c r="S17" s="31"/>
-      <c r="T17" s="33"/>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="34"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="33"/>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" s="33"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="34"/>
-      <c r="R19" s="34"/>
-      <c r="S19" s="34"/>
-      <c r="T19" s="33"/>
-    </row>
-    <row r="20" spans="1:20" s="1" customFormat="1">
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
-      <c r="L20" s="42"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42"/>
-      <c r="S20" s="42"/>
-    </row>
-    <row r="21" spans="1:20" s="1" customFormat="1">
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="42"/>
-      <c r="S21" s="42"/>
-    </row>
-    <row r="22" spans="1:20" s="1" customFormat="1">
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="L22" s="42"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="P22" s="42"/>
-      <c r="Q22" s="42"/>
-      <c r="R22" s="42"/>
-      <c r="S22" s="42"/>
+    <row r="1" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+    </row>
+    <row r="2" spans="1:19" ht="11.25" customHeight="1">
+      <c r="A2" s="54"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="45"/>
+    </row>
+    <row r="3" spans="1:19" ht="14.25" customHeight="1">
+      <c r="A3" s="55"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="46"/>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="53"/>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="41"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="42"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="43"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
+      <c r="P8" s="28"/>
+      <c r="Q8" s="28"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="42"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="43"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="39"/>
+      <c r="S10" s="44"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="37"/>
+      <c r="N11" s="37"/>
+      <c r="O11" s="37"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="43"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="42"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="43"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="42"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="37"/>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="37"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="43"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="28"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="42"/>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" s="29"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="30"/>
+      <c r="O17" s="30"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="A4:S4"/>
@@ -1431,6 +1372,12 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.98425196850393704" bottom="0.39370078740157499" header="0.39370078740157499" footer="0.31496062992126"/>

</xml_diff>